<commit_message>
Added online update function
</commit_message>
<xml_diff>
--- a/testFiles/PDF to Excel format.xlsx
+++ b/testFiles/PDF to Excel format.xlsx
@@ -519,10 +519,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A5:XFD56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
@@ -693,324 +693,2004 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr"/>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>0003638</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1,080</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2.15000</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr"/>
+      <c r="J5" s="0" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr"/>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>0003639</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1,080</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2.15000</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr"/>
+      <c r="J6" s="0" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr"/>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>0003641</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 680</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2.55000</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr"/>
+      <c r="J7" s="0" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr"/>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>0003642</t>
+        </is>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 680</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2.70000</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr"/>
+      <c r="J8" s="0" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr"/>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>0003643</t>
+        </is>
+      </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 440</t>
+        </is>
+      </c>
+      <c r="H9" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2.70000</t>
+        </is>
+      </c>
+      <c r="I9" s="0" t="inlineStr"/>
+      <c r="J9" s="0" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr"/>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>0003644</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 440</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $4.85000</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr"/>
+      <c r="J10" s="0" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr"/>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>0003645</t>
+        </is>
+      </c>
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 320</t>
+        </is>
+      </c>
+      <c r="H11" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $1.62000</t>
+        </is>
+      </c>
+      <c r="I11" s="0" t="inlineStr"/>
+      <c r="J11" s="0" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr"/>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>0003646</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 320</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $1.35000</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr"/>
+      <c r="J12" s="0" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr"/>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>0003663</t>
+        </is>
+      </c>
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1,200</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $1.62000</t>
+        </is>
+      </c>
+      <c r="I13" s="0" t="inlineStr"/>
+      <c r="J13" s="0" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr"/>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>0005567</t>
+        </is>
+      </c>
+      <c r="G14" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H14" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $59.69000</t>
+        </is>
+      </c>
+      <c r="I14" s="0" t="inlineStr"/>
+      <c r="J14" s="0" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr"/>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>0006758</t>
+        </is>
+      </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $248.72000</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr"/>
+      <c r="J15" s="0" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr"/>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>0006759</t>
+        </is>
+      </c>
+      <c r="G16" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H16" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $248.72000</t>
+        </is>
+      </c>
+      <c r="I16" s="0" t="inlineStr"/>
+      <c r="J16" s="0" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr"/>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>0007198</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $49.58000</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr"/>
+      <c r="J17" s="0" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr"/>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>0007199</t>
+        </is>
+      </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $1,027.13000</t>
+        </is>
+      </c>
+      <c r="I18" s="0" t="inlineStr"/>
+      <c r="J18" s="0" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr"/>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>0007200</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $212.54000</t>
+        </is>
+      </c>
+      <c r="I19" s="0" t="inlineStr"/>
+      <c r="J19" s="0" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr"/>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>0007209</t>
+        </is>
+      </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $63.76000</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr"/>
+      <c r="J20" s="0" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr"/>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>0007210</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $63.76000</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr"/>
+      <c r="J21" s="0" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr"/>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>PRO-101 (Update to PRO-157)</t>
+        </is>
+      </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $498.48000</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr"/>
+      <c r="J22" s="0" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr"/>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>PRO-102 (Update to PRO-159)</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $2,347.87000</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr"/>
+      <c r="J23" s="0" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr"/>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>PRO-103 (Update to PRO-158)</t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $498.48000</t>
+        </is>
+      </c>
+      <c r="I24" s="0" t="inlineStr"/>
+      <c r="J24" s="0" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr"/>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>PRO-104 (Update to PRO-160)</t>
+        </is>
+      </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $177.09000</t>
+        </is>
+      </c>
+      <c r="I25" s="0" t="inlineStr"/>
+      <c r="J25" s="0" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr"/>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>PRO-106 (Update to PRO-154)</t>
+        </is>
+      </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H26" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $1,416.73000</t>
+        </is>
+      </c>
+      <c r="I26" s="0" t="inlineStr"/>
+      <c r="J26" s="0" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr"/>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>PRO-107</t>
+        </is>
+      </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $21.26000</t>
+        </is>
+      </c>
+      <c r="I27" s="0" t="inlineStr"/>
+      <c r="J27" s="0" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr"/>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>PRO-108 (Update to PRO-153)</t>
+        </is>
+      </c>
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H28" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $498.48000</t>
+        </is>
+      </c>
+      <c r="I28" s="0" t="inlineStr"/>
+      <c r="J28" s="0" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr"/>
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>PRO-110</t>
+        </is>
+      </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H29" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $85.00000</t>
+        </is>
+      </c>
+      <c r="I29" s="0" t="inlineStr"/>
+      <c r="J29" s="0" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr"/>
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>PRO-111 (Update to PRO-150)</t>
+        </is>
+      </c>
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H30" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $920.87000</t>
+        </is>
+      </c>
+      <c r="I30" s="0" t="inlineStr"/>
+      <c r="J30" s="0" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr"/>
+      <c r="E31" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F31" s="0" t="inlineStr">
+        <is>
+          <t>PRO-112 (Update to PRO-151)</t>
+        </is>
+      </c>
+      <c r="G31" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H31" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $708.37000</t>
+        </is>
+      </c>
+      <c r="I31" s="0" t="inlineStr"/>
+      <c r="J31" s="0" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr"/>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>PRO-113 (Update to PRO-156)</t>
+        </is>
+      </c>
+      <c r="G32" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H32" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $850.04000</t>
+        </is>
+      </c>
+      <c r="I32" s="0" t="inlineStr"/>
+      <c r="J32" s="0" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr"/>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>PRO-114</t>
+        </is>
+      </c>
+      <c r="G33" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40</t>
+        </is>
+      </c>
+      <c r="H33" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $16.78000</t>
+        </is>
+      </c>
+      <c r="I33" s="0" t="inlineStr"/>
+      <c r="J33" s="0" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr"/>
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>PRO-116</t>
+        </is>
+      </c>
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H34" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $177.09000</t>
+        </is>
+      </c>
+      <c r="I34" s="0" t="inlineStr"/>
+      <c r="J34" s="0" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr"/>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>PRO-117</t>
+        </is>
+      </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H35" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $127.50000</t>
+        </is>
+      </c>
+      <c r="I35" s="0" t="inlineStr"/>
+      <c r="J35" s="0" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr"/>
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>PRO-119</t>
+        </is>
+      </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H36" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $120.43000</t>
+        </is>
+      </c>
+      <c r="I36" s="0" t="inlineStr"/>
+      <c r="J36" s="0" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr"/>
+      <c r="E37" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F37" s="0" t="inlineStr">
+        <is>
+          <t>PRO-120</t>
+        </is>
+      </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H37" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $113.23000</t>
+        </is>
+      </c>
+      <c r="I37" s="0" t="inlineStr"/>
+      <c r="J37" s="0" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr"/>
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>PRO-121</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $498.48000</t>
+        </is>
+      </c>
+      <c r="I38" s="0" t="inlineStr"/>
+      <c r="J38" s="0" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr"/>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F39" s="0" t="inlineStr">
+        <is>
+          <t>PRO-223</t>
+        </is>
+      </c>
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 80</t>
+        </is>
+      </c>
+      <c r="H39" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $67.12000</t>
+        </is>
+      </c>
+      <c r="I39" s="0" t="inlineStr"/>
+      <c r="J39" s="0" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr"/>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>PRO-235</t>
+        </is>
+      </c>
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H40" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $33.56000</t>
+        </is>
+      </c>
+      <c r="I40" s="0" t="inlineStr"/>
+      <c r="J40" s="0" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr"/>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>PRO-236</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H41" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $53.68000</t>
+        </is>
+      </c>
+      <c r="I41" s="0" t="inlineStr"/>
+      <c r="J41" s="0" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr"/>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t>PROS-001</t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40</t>
+        </is>
+      </c>
+      <c r="H42" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $187.82000</t>
+        </is>
+      </c>
+      <c r="I42" s="0" t="inlineStr"/>
+      <c r="J42" s="0" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr"/>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t>PROS-016 (Update to PROS-022)</t>
+        </is>
+      </c>
+      <c r="G43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H43" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $212.51000</t>
+        </is>
+      </c>
+      <c r="I43" s="0" t="inlineStr"/>
+      <c r="J43" s="0" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr"/>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>PROS-018 (Update to PROS-024)</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H44" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $212.51000</t>
+        </is>
+      </c>
+      <c r="I44" s="0" t="inlineStr"/>
+      <c r="J44" s="0" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr"/>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t>PROS-019 (Update to PROS-023)</t>
+        </is>
+      </c>
+      <c r="G45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 20</t>
+        </is>
+      </c>
+      <c r="H45" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $212.51000</t>
+        </is>
+      </c>
+      <c r="I45" s="0" t="inlineStr"/>
+      <c r="J45" s="0" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>2/1/2023</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>114125</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr"/>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59751-4 SHIP </t>
+        </is>
+      </c>
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t>PROS-025</t>
+        </is>
+      </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40</t>
+        </is>
+      </c>
+      <c r="H46" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> $187.82000</t>
+        </is>
+      </c>
+      <c r="I46" s="0" t="inlineStr"/>
+      <c r="J46" s="0" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>21-C30350-AB HOOD PANEL LWR 2.1 Frozen RobertoScarati</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>21-C31100-AA HOOD REAR TRIM ASSY 1.1 Frozen EdoardoFavata</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>21-C36050-AB CENTRAL SUPPORT BRACKET 2.1 Frozen RobertoScarati.</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>21-C37000-AB DECO TRIM, FRONT FASCIA UPPER 2.1 Frozen RobertoScarati.</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>21-C38100-AB NOSE BLACK INSERT 2.1 Frozen RobertoScarati.</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>P21-C96110-AA FENDER APPLIQUE LH-ASSY</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>P21-C96120-AA FENDER APPLIQUE RH-ASSY</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G53" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
         <is>
           <t>2/10/2023</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MTC</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MTC</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
         <is>
           <t>114248</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
         <is>
           <t xml:space="preserve">P_515111 SHIP </t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>P21-C96120-AA FENDER APPLIQUE RH-ASSY</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G54" t="inlineStr">
         <is>
           <t xml:space="preserve"> 40</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H54" t="inlineStr">
         <is>
           <t xml:space="preserve"> $153.92100</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>